<commit_message>
Checking coomit throgh VS
</commit_message>
<xml_diff>
--- a/SMS_Database.xlsx
+++ b/SMS_Database.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22527"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pande\Downloads\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5606E4B2-B4C7-4979-84C6-D40EB7A2BD0F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
   </bookViews>
   <sheets>
     <sheet name="SignupAndLogin" sheetId="1" r:id="rId1"/>
@@ -22,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="64">
   <si>
     <t>UserID</t>
   </si>
@@ -208,13 +202,19 @@
   </si>
   <si>
     <t>INT(4)</t>
+  </si>
+  <si>
+    <t>FirstTime Given by US</t>
+  </si>
+  <si>
+    <t>Comments</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -343,7 +343,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -375,27 +375,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -427,24 +409,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -620,14 +584,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B3:E39"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="B3:F39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+      <selection activeCell="F3" sqref="F3:F24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="4"/>
     <col min="2" max="2" width="23.5703125" style="4" bestFit="1" customWidth="1"/>
@@ -641,15 +605,18 @@
     <col min="11" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:6" s="1" customFormat="1">
       <c r="B3" s="5" t="s">
         <v>57</v>
       </c>
       <c r="C3" s="5"/>
       <c r="D3" s="5"/>
       <c r="E3" s="5"/>
-    </row>
-    <row r="4" spans="2:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="F3" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6" s="1" customFormat="1">
       <c r="B4" s="2" t="s">
         <v>41</v>
       </c>
@@ -662,8 +629,9 @@
       <c r="E4" s="2" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F4" s="2"/>
+    </row>
+    <row r="5" spans="2:6" ht="30">
       <c r="B5" s="3" t="s">
         <v>0</v>
       </c>
@@ -676,8 +644,11 @@
       <c r="E5" s="3" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="6" spans="2:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="F5" s="3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" ht="45">
       <c r="B6" s="3" t="s">
         <v>11</v>
       </c>
@@ -690,8 +661,9 @@
       <c r="E6" s="3" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F6" s="3"/>
+    </row>
+    <row r="7" spans="2:6">
       <c r="B7" s="3" t="s">
         <v>1</v>
       </c>
@@ -704,8 +676,9 @@
       <c r="E7" s="3" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F7" s="3"/>
+    </row>
+    <row r="8" spans="2:6">
       <c r="B8" s="3" t="s">
         <v>3</v>
       </c>
@@ -716,8 +689,9 @@
       <c r="E8" s="3" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F8" s="3"/>
+    </row>
+    <row r="9" spans="2:6">
       <c r="B9" s="3" t="s">
         <v>2</v>
       </c>
@@ -730,8 +704,9 @@
       <c r="E9" s="3" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F9" s="3"/>
+    </row>
+    <row r="10" spans="2:6">
       <c r="B10" s="3" t="s">
         <v>4</v>
       </c>
@@ -744,8 +719,9 @@
       <c r="E10" s="3" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F10" s="3"/>
+    </row>
+    <row r="11" spans="2:6">
       <c r="B11" s="3" t="s">
         <v>5</v>
       </c>
@@ -756,8 +732,9 @@
       <c r="E11" s="3" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F11" s="3"/>
+    </row>
+    <row r="12" spans="2:6">
       <c r="B12" s="3" t="s">
         <v>6</v>
       </c>
@@ -768,8 +745,9 @@
       <c r="E12" s="3" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F12" s="3"/>
+    </row>
+    <row r="13" spans="2:6">
       <c r="B13" s="3" t="s">
         <v>7</v>
       </c>
@@ -780,8 +758,9 @@
       <c r="E13" s="3" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F13" s="3"/>
+    </row>
+    <row r="14" spans="2:6">
       <c r="B14" s="3" t="s">
         <v>8</v>
       </c>
@@ -794,8 +773,9 @@
       <c r="E14" s="3" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F14" s="3"/>
+    </row>
+    <row r="15" spans="2:6">
       <c r="B15" s="3" t="s">
         <v>9</v>
       </c>
@@ -808,8 +788,9 @@
       <c r="E15" s="3" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F15" s="3"/>
+    </row>
+    <row r="16" spans="2:6">
       <c r="B16" s="3" t="s">
         <v>10</v>
       </c>
@@ -822,8 +803,9 @@
       <c r="E16" s="3" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F16" s="3"/>
+    </row>
+    <row r="17" spans="2:6">
       <c r="B17" s="3" t="s">
         <v>60</v>
       </c>
@@ -834,8 +816,9 @@
       <c r="E17" s="3" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F17" s="3"/>
+    </row>
+    <row r="18" spans="2:6">
       <c r="B18" s="3" t="s">
         <v>13</v>
       </c>
@@ -846,8 +829,9 @@
       <c r="E18" s="3" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F18" s="3"/>
+    </row>
+    <row r="19" spans="2:6">
       <c r="B19" s="3" t="s">
         <v>59</v>
       </c>
@@ -858,8 +842,9 @@
       <c r="E19" s="3" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F19" s="3"/>
+    </row>
+    <row r="20" spans="2:6">
       <c r="B20" s="3" t="s">
         <v>58</v>
       </c>
@@ -870,8 +855,9 @@
       <c r="E20" s="3" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F20" s="3"/>
+    </row>
+    <row r="21" spans="2:6">
       <c r="B21" s="3" t="s">
         <v>15</v>
       </c>
@@ -884,8 +870,9 @@
       <c r="E21" s="3" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F21" s="3"/>
+    </row>
+    <row r="22" spans="2:6">
       <c r="B22" s="3" t="s">
         <v>16</v>
       </c>
@@ -898,8 +885,9 @@
       <c r="E22" s="3" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F22" s="3"/>
+    </row>
+    <row r="23" spans="2:6">
       <c r="B23" s="3" t="s">
         <v>35</v>
       </c>
@@ -910,8 +898,9 @@
       <c r="E23" s="3" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F23" s="3"/>
+    </row>
+    <row r="24" spans="2:6">
       <c r="B24" s="3" t="s">
         <v>36</v>
       </c>
@@ -922,8 +911,9 @@
       <c r="E24" s="3" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F24" s="3"/>
+    </row>
+    <row r="26" spans="2:6">
       <c r="B26" s="5" t="s">
         <v>19</v>
       </c>
@@ -931,7 +921,7 @@
       <c r="D26" s="5"/>
       <c r="E26" s="5"/>
     </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:6">
       <c r="B27" s="2" t="s">
         <v>41</v>
       </c>
@@ -945,7 +935,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:6">
       <c r="B28" s="3" t="s">
         <v>26</v>
       </c>
@@ -957,7 +947,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:6">
       <c r="B29" s="3" t="s">
         <v>0</v>
       </c>
@@ -969,7 +959,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="30" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:6">
       <c r="B30" s="3" t="s">
         <v>11</v>
       </c>
@@ -983,7 +973,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="31" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:6">
       <c r="B31" s="3" t="s">
         <v>17</v>
       </c>
@@ -997,7 +987,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="32" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:6">
       <c r="B32" s="3" t="s">
         <v>18</v>
       </c>
@@ -1011,7 +1001,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="33" spans="2:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:5" ht="45">
       <c r="B33" s="3" t="s">
         <v>52</v>
       </c>
@@ -1023,7 +1013,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="34" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:5" ht="30">
       <c r="B34" s="3" t="s">
         <v>33</v>
       </c>
@@ -1037,7 +1027,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="35" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:5" ht="30">
       <c r="B35" s="3" t="s">
         <v>32</v>
       </c>
@@ -1051,7 +1041,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="36" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:5">
       <c r="B36" s="3" t="s">
         <v>12</v>
       </c>
@@ -1065,7 +1055,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="37" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:5">
       <c r="B37" s="3" t="s">
         <v>14</v>
       </c>
@@ -1079,7 +1069,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="38" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:5">
       <c r="B38" s="3" t="s">
         <v>34</v>
       </c>
@@ -1093,7 +1083,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="39" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:5">
       <c r="B39" s="3" t="s">
         <v>38</v>
       </c>
@@ -1118,24 +1108,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>